<commit_message>
se finaliza registro en ios
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/registro/RegistroUsuario.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/registro/RegistroUsuario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -119,9 +119,6 @@
     <t>95400152</t>
   </si>
   <si>
-    <t>sandrita69</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
@@ -137,22 +134,29 @@
     <t>CONSULTAR_PRODUCTO</t>
   </si>
   <si>
-    <t>10757880</t>
-  </si>
-  <si>
-    <t>pruebasqa93</t>
+    <t>10757881</t>
+  </si>
+  <si>
+    <t>pruebasqa94</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -238,22 +242,23 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -559,7 +564,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -620,7 +625,7 @@
         <v>13</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -667,7 +672,7 @@
         <v>25</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -675,13 +680,13 @@
         <v>26</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>27</v>
@@ -708,27 +713,27 @@
         <v>23</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>25</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="13" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>31</v>
+      <c r="D4" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>27</v>
@@ -740,10 +745,10 @@
         <v>28</v>
       </c>
       <c r="H4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>21</v>
@@ -757,7 +762,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
finaliza transaccion registro en Android
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/registro/RegistroUsuario.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/registro/RegistroUsuario.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -67,16 +67,13 @@
     <t>10757881</t>
   </si>
   <si>
-    <t>10757880</t>
-  </si>
-  <si>
     <t>1234</t>
   </si>
   <si>
     <t>4321</t>
   </si>
   <si>
-    <t>Alterno</t>
+    <t>Acierto</t>
   </si>
   <si>
     <t>000</t>
@@ -94,28 +91,25 @@
     <t>ACTIVO</t>
   </si>
   <si>
-    <t>pruebasqa99</t>
+    <t>pruebasqar99</t>
   </si>
   <si>
     <t>jalzate@todo1.net</t>
   </si>
   <si>
+    <t>CONSULTAR_PRODUCTO</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>10757882</t>
+  </si>
+  <si>
+    <t>pruebasqar94</t>
+  </si>
+  <si>
     <t>EPREPAGO</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>10757882</t>
-  </si>
-  <si>
-    <t>Acierto</t>
-  </si>
-  <si>
-    <t>pruebasqa94</t>
-  </si>
-  <si>
-    <t>CONSULTAR_PRODUCTO</t>
   </si>
   <si>
     <t>3</t>
@@ -143,10 +137,10 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,13 +163,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,28 +187,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -235,16 +209,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -252,7 +249,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -273,56 +270,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -355,31 +342,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -392,150 +523,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -564,24 +551,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -599,26 +568,42 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -639,32 +624,34 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -682,148 +669,146 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="10" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="10" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1174,8 +1159,8 @@
   <sheetPr/>
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16190476190476" defaultRowHeight="15"/>
@@ -1223,10 +1208,10 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -1235,192 +1220,192 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="M2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="N2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="N3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:15">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="I4" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="L4" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>25</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-      <c r="O4" s="10" t="s">
-        <v>33</v>
+      <c r="O4" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:15">
-      <c r="A5" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="A5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="15" t="s">
+      <c r="D5" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="G5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="12" t="s">
+      <c r="H5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="L5" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>25</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="10" t="s">
-        <v>33</v>
+      <c r="O5" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="13:13">
-      <c r="M14" s="11"/>
+      <c r="M14" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Estabilizacion de transacciones entregadas por data, codigo, mapeo
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/registro/RegistroUsuario.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/registro/RegistroUsuario.xlsx
@@ -1,30 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/ProyectosTODO1/bancolombia-app-personas-osp-tests-bdd-screen-play/APP_PERSONAS/src/test/resources/datadriven/registro/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20520" yWindow="3420" windowWidth="10000" windowHeight="13760"/>
+    <workbookView windowWidth="20490" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -74,6 +64,12 @@
     <t>1</t>
   </si>
   <si>
+    <t>700102</t>
+  </si>
+  <si>
+    <t>700100</t>
+  </si>
+  <si>
     <t>1234</t>
   </si>
   <si>
@@ -98,6 +94,9 @@
     <t>ACTIVO</t>
   </si>
   <si>
+    <t>autouser15</t>
+  </si>
+  <si>
     <t>jalzate@todo1.net</t>
   </si>
   <si>
@@ -107,12 +106,24 @@
     <t>2</t>
   </si>
   <si>
+    <t>700103</t>
+  </si>
+  <si>
+    <t>700101</t>
+  </si>
+  <si>
     <t>EPREPAGO</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
+    <t>22480139</t>
+  </si>
+  <si>
+    <t>48313974</t>
+  </si>
+  <si>
     <t>001</t>
   </si>
   <si>
@@ -122,41 +133,28 @@
     <t>4</t>
   </si>
   <si>
-    <t>700100</t>
-  </si>
-  <si>
-    <t>pruebasregistro48</t>
-  </si>
-  <si>
-    <t>700101</t>
-  </si>
-  <si>
-    <t>pruebasregistro49</t>
+    <t>87576487</t>
   </si>
   <si>
     <t>22493944</t>
-  </si>
-  <si>
-    <t>48313974</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -189,8 +187,144 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,8 +349,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -239,39 +559,321 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="10" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -320,7 +922,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -355,7 +957,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -558,26 +1160,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="13" max="13" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.8285714285714" customWidth="1"/>
+    <col min="14" max="14" width="15" customWidth="1"/>
+    <col min="15" max="15" width="19.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" ht="15.75" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -608,10 +1210,10 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -620,194 +1222,195 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:15">
+      <c r="A2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="11" t="s">
+    </row>
+    <row r="4" ht="15.75" spans="1:15">
+      <c r="A4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="D4" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="F4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="G4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="11" t="s">
+      <c r="H4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="7" t="s">
+      <c r="K4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="L4" s="11" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>23</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-      <c r="O4" s="8" t="s">
+      <c r="O4" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" spans="1:15">
+      <c r="A5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="11" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>23</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="8" t="s">
-        <v>25</v>
+      <c r="O5" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="M14" s="9"/>
+    <row r="14" spans="13:13">
+      <c r="M14" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>